<commit_message>
added b.Unit Token as a separate rfa
</commit_message>
<xml_diff>
--- a/sandbox/Yield Matrix.xlsx
+++ b/sandbox/Yield Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>TOTAL</t>
   </si>
@@ -51,6 +51,36 @@
   </si>
   <si>
     <t>Rentable Per Type</t>
+  </si>
+  <si>
+    <t>1 Bedroom + Den</t>
+  </si>
+  <si>
+    <t>2 Bedroom</t>
+  </si>
+  <si>
+    <t>Open 1 Bedroom</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Bedrooms</t>
+  </si>
+  <si>
+    <t>Baths</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
   </si>
 </sst>
 </file>
@@ -674,7 +704,7 @@
   <dimension ref="A1:CD35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,15 +732,15 @@
       </c>
       <c r="B2" s="27" t="str">
         <f>IF(UnitSummary!B1&lt;&gt;"",UnitSummary!B1,"")</f>
-        <v/>
+        <v>Open 1 Bedroom</v>
       </c>
       <c r="C2" s="27" t="str">
         <f>IF(UnitSummary!C1&lt;&gt;"",UnitSummary!C1,"")</f>
-        <v/>
+        <v>1 Bedroom + Den</v>
       </c>
       <c r="D2" s="27" t="str">
         <f>IF(UnitSummary!D1&lt;&gt;"",UnitSummary!D1,"")</f>
-        <v/>
+        <v>2 Bedroom</v>
       </c>
       <c r="E2" s="27" t="str">
         <f>IF(UnitSummary!E1&lt;&gt;"",UnitSummary!E1,"")</f>
@@ -780,23 +810,23 @@
     <row r="3" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="str">
         <f>IF(UnitSummary!A6&lt;&gt;"",UnitSummary!A6,"")</f>
-        <v/>
-      </c>
-      <c r="B3" s="22" t="str">
+        <v>FLOOR</v>
+      </c>
+      <c r="B3" s="22">
         <f>IF(UnitSummary!B6&lt;&gt;"",UnitSummary!B6,"")</f>
-        <v/>
-      </c>
-      <c r="C3" s="22" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="22">
         <f>IF(UnitSummary!C6&lt;&gt;"",UnitSummary!C6,"")</f>
-        <v/>
-      </c>
-      <c r="D3" s="22" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="D3" s="22">
         <f>IF(UnitSummary!D6&lt;&gt;"",UnitSummary!D6,"")</f>
-        <v/>
+        <v>2.1</v>
       </c>
       <c r="E3" s="22" t="str">
         <f>IF(UnitSummary!E6&lt;&gt;"",UnitSummary!E6,"")</f>
-        <v/>
+        <v>TOTAL</v>
       </c>
       <c r="F3" s="22" t="str">
         <f>IF(UnitSummary!F6&lt;&gt;"",UnitSummary!F6,"")</f>
@@ -862,23 +892,23 @@
     <row r="4" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>IF(UnitSummary!A7&lt;&gt;"",UnitSummary!A7,"")</f>
-        <v/>
-      </c>
-      <c r="B4" s="2" t="str">
+        <v>Level 1</v>
+      </c>
+      <c r="B4" s="2">
         <f>IF(UnitSummary!B7&lt;&gt;"",UnitSummary!B7,"")</f>
-        <v/>
-      </c>
-      <c r="C4" s="2" t="str">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
         <f>IF(UnitSummary!C7&lt;&gt;"",UnitSummary!C7,"")</f>
-        <v/>
-      </c>
-      <c r="D4" s="2" t="str">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
         <f>IF(UnitSummary!D7&lt;&gt;"",UnitSummary!D7,"")</f>
-        <v/>
-      </c>
-      <c r="E4" s="2" t="str">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
         <f>IF(UnitSummary!E7&lt;&gt;"",UnitSummary!E7,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>IF(UnitSummary!F7&lt;&gt;"",UnitSummary!F7,"")</f>
@@ -944,23 +974,23 @@
     <row r="5" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="str">
         <f>IF(UnitSummary!A8&lt;&gt;"",UnitSummary!A8,"")</f>
-        <v/>
-      </c>
-      <c r="B5" s="39" t="str">
+        <v>Level 2</v>
+      </c>
+      <c r="B5" s="39">
         <f>IF(UnitSummary!B8&lt;&gt;"",UnitSummary!B8,"")</f>
-        <v/>
-      </c>
-      <c r="C5" s="39" t="str">
+        <v>5</v>
+      </c>
+      <c r="C5" s="39">
         <f>IF(UnitSummary!C8&lt;&gt;"",UnitSummary!C8,"")</f>
-        <v/>
-      </c>
-      <c r="D5" s="39" t="str">
+        <v>2</v>
+      </c>
+      <c r="D5" s="39">
         <f>IF(UnitSummary!D8&lt;&gt;"",UnitSummary!D8,"")</f>
-        <v/>
-      </c>
-      <c r="E5" s="39" t="str">
+        <v>2</v>
+      </c>
+      <c r="E5" s="39">
         <f>IF(UnitSummary!E8&lt;&gt;"",UnitSummary!E8,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="F5" s="39" t="str">
         <f>IF(UnitSummary!F8&lt;&gt;"",UnitSummary!F8,"")</f>
@@ -3681,21 +3711,21 @@
       <c r="A24" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="25" t="str">
+      <c r="B24" s="25">
         <f t="shared" ref="B24:T24" si="0">IF(SUM(B4:B23)&lt;&gt;0,SUM(B4:B23),"")</f>
-        <v/>
-      </c>
-      <c r="C24" s="25" t="str">
+        <v>10</v>
+      </c>
+      <c r="C24" s="25">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D24" s="25" t="str">
+        <v>4</v>
+      </c>
+      <c r="D24" s="25">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E24" s="25" t="str">
+        <v>4</v>
+      </c>
+      <c r="E24" s="25">
         <f t="shared" si="0"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="F24" s="25" t="str">
         <f t="shared" si="0"/>
@@ -3762,17 +3792,17 @@
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="15" t="str">
+      <c r="B25" s="15">
         <f>IF(UnitSummary!B2&lt;&gt;"",UnitSummary!B2,"")</f>
-        <v/>
-      </c>
-      <c r="C25" s="15" t="str">
+        <v>200</v>
+      </c>
+      <c r="C25" s="15">
         <f>IF(UnitSummary!C2&lt;&gt;"",UnitSummary!C2,"")</f>
-        <v/>
-      </c>
-      <c r="D25" s="15" t="str">
+        <v>300</v>
+      </c>
+      <c r="D25" s="15">
         <f>IF(UnitSummary!D2&lt;&gt;"",UnitSummary!D2,"")</f>
-        <v/>
+        <v>400</v>
       </c>
       <c r="E25" s="15" t="str">
         <f>IF(UnitSummary!E2&lt;&gt;"",UnitSummary!E2,"")</f>
@@ -3832,17 +3862,17 @@
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="7" t="e">
+      <c r="B26" s="7">
         <f>B24/B29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C26" s="7" t="e">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C26" s="7">
         <f>C24/B29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D26" s="7" t="e">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D26" s="7">
         <f>D24/B29</f>
-        <v>#VALUE!</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -3866,17 +3896,17 @@
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="11" t="e">
+      <c r="B27" s="11">
         <f>B25*B24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C27" s="11" t="e">
+        <v>2000</v>
+      </c>
+      <c r="C27" s="11">
         <f t="shared" ref="C27:D27" si="1">C25*C24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D27" s="11" t="e">
+        <v>1200</v>
+      </c>
+      <c r="D27" s="11">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1600</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -3923,18 +3953,18 @@
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="29" t="str">
+      <c r="B29" s="29">
         <f>E24</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="32" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="13"/>
-      <c r="F29" s="9" t="e">
+      <c r="F29" s="9">
         <f>B30/B29</f>
-        <v>#VALUE!</v>
+        <v>266.66666666666669</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -3956,9 +3986,9 @@
       <c r="A30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="30" t="e">
+      <c r="B30" s="30">
         <f>SUM(27:27)</f>
-        <v>#VALUE!</v>
+        <v>4800</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -3991,15 +4021,15 @@
       </c>
       <c r="B32" s="44" t="str">
         <f>IF(UnitMix!A1&lt;&gt;"",UnitMix!A1,"")</f>
-        <v/>
+        <v>1 Bedroom + Den</v>
       </c>
       <c r="C32" s="47" t="str">
         <f>IF(UnitMix!B1&lt;&gt;"",UnitMix!B1,"")</f>
-        <v/>
+        <v>2 Bedroom</v>
       </c>
       <c r="D32" s="50" t="str">
         <f>IF(UnitMix!C1&lt;&gt;"",UnitMix!C1,"")</f>
-        <v/>
+        <v>Open 1 Bedroom</v>
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="43"/>
@@ -4049,17 +4079,17 @@
       </c>
     </row>
     <row r="33" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="45" t="str">
+      <c r="B33" s="45">
         <f>IF(UnitMix!A2&lt;&gt;"",UnitMix!A2,"")</f>
-        <v/>
-      </c>
-      <c r="C33" s="48" t="str">
+        <v>4</v>
+      </c>
+      <c r="C33" s="48">
         <f>IF(UnitMix!B2&lt;&gt;"",UnitMix!B2,"")</f>
-        <v/>
-      </c>
-      <c r="D33" s="51" t="str">
+        <v>4</v>
+      </c>
+      <c r="D33" s="51">
         <f>IF(UnitMix!C2&lt;&gt;"",UnitMix!C2,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="E33" s="33" t="str">
         <f>IF(UnitMix!D2&lt;&gt;"",UnitMix!D2,"")</f>
@@ -4128,17 +4158,17 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="46" t="e">
+      <c r="B34" s="46">
         <f>B33/B29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C34" s="49" t="e">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="C34" s="49">
         <f>C33/B29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D34" s="52" t="e">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D34" s="52">
         <f>D33/B29</f>
-        <v>#VALUE!</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="37"/>
@@ -4173,28 +4203,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="A1:G11"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C6">
+        <v>1.2</v>
+      </c>
+      <c r="D6">
+        <v>2.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>